<commit_message>
Increased the size of legends
</commit_message>
<xml_diff>
--- a/N uptake/N_uptake_maturity/0N_Nuptake_By_Year.xlsx
+++ b/N uptake/N_uptake_maturity/0N_Nuptake_By_Year.xlsx
@@ -416,19 +416,19 @@
         </is>
       </c>
       <c r="C2">
-        <v>59.92719648436591</v>
+        <v>59.92719648436582</v>
       </c>
       <c r="D2">
-        <v>8.327014507379953</v>
+        <v>8.327014506708313</v>
       </c>
       <c r="E2">
-        <v>12.58127128580334</v>
+        <v>12.58127128962635</v>
       </c>
       <c r="F2">
-        <v>41.87672345610804</v>
+        <v>41.87672345814161</v>
       </c>
       <c r="G2">
-        <v>77.97766951262379</v>
+        <v>77.97766951059003</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -451,19 +451,19 @@
         </is>
       </c>
       <c r="C3">
-        <v>85.60446469065033</v>
+        <v>85.60446469065015</v>
       </c>
       <c r="D3">
-        <v>8.327014507379957</v>
+        <v>8.327014506708304</v>
       </c>
       <c r="E3">
-        <v>12.58127128580331</v>
+        <v>12.58127128962627</v>
       </c>
       <c r="F3">
-        <v>67.55399166239243</v>
+        <v>67.55399166442595</v>
       </c>
       <c r="G3">
-        <v>103.6549377189082</v>
+        <v>103.6549377168743</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>66.42947907953436</v>
+        <v>66.42947907953442</v>
       </c>
       <c r="D4">
         <v>11.92667576821407</v>
@@ -495,10 +495,10 @@
         <v>16.90496631949647</v>
       </c>
       <c r="F4">
-        <v>41.25561271077014</v>
+        <v>41.25561271077019</v>
       </c>
       <c r="G4">
-        <v>91.60334544829858</v>
+        <v>91.60334544829865</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -521,16 +521,16 @@
         </is>
       </c>
       <c r="C5">
-        <v>98.01028182111391</v>
+        <v>98.01028182111389</v>
       </c>
       <c r="D5">
-        <v>11.92667576821402</v>
+        <v>11.92667576821403</v>
       </c>
       <c r="E5">
-        <v>16.90496631949619</v>
+        <v>16.90496631949621</v>
       </c>
       <c r="F5">
-        <v>72.83641545234975</v>
+        <v>72.83641545234973</v>
       </c>
       <c r="G5">
         <v>123.1841481898781</v>
@@ -556,19 +556,19 @@
         </is>
       </c>
       <c r="C6">
-        <v>56.11176397560631</v>
+        <v>56.11176397560685</v>
       </c>
       <c r="D6">
-        <v>12.67476398655016</v>
+        <v>12.67476398655031</v>
       </c>
       <c r="E6">
-        <v>23.70423007212035</v>
+        <v>23.70423007211963</v>
       </c>
       <c r="F6">
-        <v>29.9350530044173</v>
+        <v>29.93505300441748</v>
       </c>
       <c r="G6">
-        <v>82.28847494679532</v>
+        <v>82.28847494679621</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -591,19 +591,19 @@
         </is>
       </c>
       <c r="C7">
-        <v>93.57271822609043</v>
+        <v>93.57271822609036</v>
       </c>
       <c r="D7">
-        <v>12.67476398655021</v>
+        <v>12.67476398655031</v>
       </c>
       <c r="E7">
-        <v>23.70423007212018</v>
+        <v>23.7042300721196</v>
       </c>
       <c r="F7">
-        <v>67.39600725490131</v>
+        <v>67.39600725490099</v>
       </c>
       <c r="G7">
-        <v>119.7494291972796</v>
+        <v>119.7494291972797</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -626,19 +626,19 @@
         </is>
       </c>
       <c r="C8">
-        <v>60.82281317983561</v>
+        <v>60.82281317983503</v>
       </c>
       <c r="D8">
-        <v>6.02772336464519</v>
+        <v>6.027723364645365</v>
       </c>
       <c r="E8">
-        <v>70.76988316721602</v>
+        <v>70.76988316720744</v>
       </c>
       <c r="F8">
-        <v>48.80319686730462</v>
+        <v>48.80319686730366</v>
       </c>
       <c r="G8">
-        <v>72.84242949236661</v>
+        <v>72.84242949236639</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -661,19 +661,19 @@
         </is>
       </c>
       <c r="C9">
-        <v>92.39582157928473</v>
+        <v>92.3958215792847</v>
       </c>
       <c r="D9">
-        <v>6.027723364645185</v>
+        <v>6.027723364645372</v>
       </c>
       <c r="E9">
-        <v>70.769883167218</v>
+        <v>70.76988316720612</v>
       </c>
       <c r="F9">
-        <v>80.37620526675374</v>
+        <v>80.37620526675332</v>
       </c>
       <c r="G9">
-        <v>104.4154378918157</v>
+        <v>104.4154378918161</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>

</xml_diff>